<commit_message>
add TU Delft CS. Fine tune EE, CS, ME
</commit_message>
<xml_diff>
--- a/database/ComputerScience/CS_Programs.xlsx
+++ b/database/ComputerScience/CS_Programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ComputerScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25129A9C-98BD-4674-A2DF-E9F8DA4F11EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FE560A-6F2D-4BFA-A7FE-F46A3C097549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program_choosing" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Program</t>
   </si>
@@ -48,7 +48,10 @@
     <t>TUM_Informatics</t>
   </si>
   <si>
-    <t>TU Data Engineering and Analytics</t>
+    <t>TUM Data Engineering and Analytics</t>
+  </si>
+  <si>
+    <t>TU Delft Computer Science</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,9 +428,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B6" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B7" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
improve keywords. Add ECTS conversion by the factor of 1.5
</commit_message>
<xml_diff>
--- a/database/ComputerScience/CS_Programs.xlsx
+++ b/database/ComputerScience/CS_Programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ComputerScience\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c520cbcd5c1ba828/20110706/TaiGer_Transcript-Program_Comparer/database/ComputerScience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FE560A-6F2D-4BFA-A7FE-F46A3C097549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{74FE560A-6F2D-4BFA-A7FE-F46A3C097549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3043A9A-8158-43E5-A011-ADC033FF130D}"/>
   <bookViews>
-    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program_choosing" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Program</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>TU Delft Computer Science</t>
+  </si>
+  <si>
+    <t>RWTH_Aachen_DDS</t>
+  </si>
+  <si>
+    <t>RWTH_Aachen_TIME</t>
+  </si>
+  <si>
+    <t>Uni_Goettingen_Applied_CS</t>
   </si>
 </sst>
 </file>
@@ -369,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,9 +445,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B7" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B10" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add RWTH Software System Eng, and RWTH Media Informatics
</commit_message>
<xml_diff>
--- a/database/ComputerScience/CS_Programs.xlsx
+++ b/database/ComputerScience/CS_Programs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c520cbcd5c1ba828/20110706/TaiGer_Transcript-Program_Comparer/database/ComputerScience/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ComputerScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{74FE560A-6F2D-4BFA-A7FE-F46A3C097549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3043A9A-8158-43E5-A011-ADC033FF130D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702FB0C2-686F-4396-9D33-50C9C89A760C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Program</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Uni_Goettingen_Applied_CS</t>
+  </si>
+  <si>
+    <t>RWTH_Aachen_Software_System_Engineering</t>
+  </si>
+  <si>
+    <t>RWTH_Aachen_Media_Informatics</t>
   </si>
 </sst>
 </file>
@@ -378,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -415,7 +421,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -423,7 +429,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -431,7 +437,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -439,7 +445,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -447,7 +453,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -455,7 +461,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -463,15 +469,31 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B10" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B12" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add uploading generated file to S3. reading transcript excel input from S3 not implemented yet
</commit_message>
<xml_diff>
--- a/database/ComputerScience/CS_Programs.xlsx
+++ b/database/ComputerScience/CS_Programs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ComputerScience\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c520cbcd5c1ba828/20110706/TaiGer_Transcript-Program_Comparer/database/ComputerScience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702FB0C2-686F-4396-9D33-50C9C89A760C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{702FB0C2-686F-4396-9D33-50C9C89A760C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25C89AE2-DCC8-471F-8D23-2AA1108E54FE}"/>
   <bookViews>
     <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Program</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>RWTH_Aachen_Data Science</t>
-  </si>
-  <si>
     <t>Freie Uni Berlin - Data Science</t>
   </si>
   <si>
@@ -67,6 +64,18 @@
   </si>
   <si>
     <t>RWTH_Aachen_Media_Informatics</t>
+  </si>
+  <si>
+    <t>TUM_Math_Data_Science_MathBackground</t>
+  </si>
+  <si>
+    <t>TUM_Math_Data_Science_CSBackground</t>
+  </si>
+  <si>
+    <t>RWTH_Aachen_Data Science_CS_BG</t>
+  </si>
+  <si>
+    <t>RWTH_Aachen_Data Science_Math_BG</t>
   </si>
 </sst>
 </file>
@@ -384,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,7 +414,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -413,7 +422,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -421,7 +430,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -429,7 +438,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -437,7 +446,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -445,7 +454,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -453,7 +462,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -461,7 +470,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -469,7 +478,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -477,7 +486,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -485,15 +494,39 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B12" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B15" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>